<commit_message>
chore: fix the Motors notes
</commit_message>
<xml_diff>
--- a/motors/comms_re.xlsx
+++ b/motors/comms_re.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t xml:space="preserve">Motor command buffer (sent by main MCU) - Start Motor (step 1)</t>
   </si>
@@ -45,6 +45,12 @@
     <t>header[0]</t>
   </si>
   <si>
+    <t>motor_id</t>
+  </si>
+  <si>
+    <t>command_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">Motor command buffer (sent by main MCU) - Start Motor (step 2)</t>
   </si>
   <si>
@@ -69,9 +75,6 @@
     <t>C4</t>
   </si>
   <si>
-    <t>motor_id</t>
-  </si>
-  <si>
     <t>checksum</t>
   </si>
   <si>
@@ -93,7 +96,7 @@
     <t>27</t>
   </si>
   <si>
-    <t xml:space="preserve">motor_id ?</t>
+    <t>command_id?</t>
   </si>
   <si>
     <t>current[1]</t>
@@ -174,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -184,7 +187,6 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -705,7 +707,7 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="14.57421875"/>
-    <col customWidth="1" min="6" max="6" width="10.8515625"/>
+    <col customWidth="1" min="6" max="6" width="14.00390625"/>
     <col bestFit="1" min="8" max="8" width="10.7109375"/>
   </cols>
   <sheetData>
@@ -811,20 +813,22 @@
       <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4"/>
       <c r="J4" s="2"/>
-      <c r="K4"/>
       <c r="L4" s="2"/>
     </row>
     <row r="5" ht="14.25"/>
     <row r="6" ht="14.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -924,9 +928,13 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -937,7 +945,7 @@
     <row r="10" ht="14.25"/>
     <row r="11" ht="14.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1006,13 +1014,13 @@
         <v>5</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>5</v>
@@ -1037,9 +1045,13 @@
       <c r="C14" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1050,7 +1062,7 @@
     <row r="15" ht="14.25"/>
     <row r="16" ht="14.25">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1112,29 +1124,29 @@
       <c r="C18" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>5</v>
@@ -1150,24 +1162,27 @@
       <c r="C19" t="s">
         <v>9</v>
       </c>
-      <c r="F19" t="s">
-        <v>18</v>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="H19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" ht="14.25"/>
     <row r="21" ht="14.25"/>
     <row r="22" ht="14.25">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1233,16 +1248,16 @@
         <v>5</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" t="s">
         <v>16</v>
       </c>
-      <c r="F24" t="s">
-        <v>14</v>
-      </c>
       <c r="G24" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>5</v>
@@ -1251,10 +1266,10 @@
         <v>5</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" ht="14.25">
@@ -1267,34 +1282,36 @@
       <c r="C25" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" t="s">
-        <v>19</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>27</v>
+      <c r="I25" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="J25" s="2"/>
-      <c r="K25" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="L25" s="6" t="s">
+      <c r="K25" s="2" t="s">
         <v>29</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="27" ht="14.25"/>
     <row r="28" ht="14.25">
       <c r="A28" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1360,28 +1377,28 @@
         <v>5</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I30" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="J30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L30" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" ht="14.25">
@@ -1396,31 +1413,31 @@
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" t="s">
         <v>20</v>
       </c>
-      <c r="F31" t="s">
-        <v>26</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>34</v>
+      <c r="I31" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="J31" s="2"/>
-      <c r="K31" s="6" t="s">
-        <v>28</v>
+      <c r="K31" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" ht="14.25">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1488,26 +1505,26 @@
       <c r="E35" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="7" t="s">
-        <v>36</v>
+      <c r="F35" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I35" t="s">
         <v>5</v>
       </c>
-      <c r="J35" s="7" t="s">
-        <v>38</v>
+      <c r="J35" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>5</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" ht="14.25">
@@ -1522,16 +1539,18 @@
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+      <c r="F36" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="G36" s="2"/>
       <c r="H36" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-      <c r="L36" s="6" t="s">
-        <v>29</v>
+      <c r="L36" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="38" ht="14.25"/>

</xml_diff>